<commit_message>
[Modify] D55060/ 55060 templates/ W50073/ W55060 by Lukas
</commit_message>
<xml_diff>
--- a/PhoenixCI/Excel_Template/55060MM.xlsx
+++ b/PhoenixCI/Excel_Template/55060MM.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Source\Repos\buckblader\RekindlePhoenixCI\PhoenixCI\Excel_Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\RekindlePhoenixCI\PhoenixCI\Excel_Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E845FD21-23B9-40FC-AB0D-C7707B48B880}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9DFDC0A5-A354-48AC-8523-046B1534BB42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
+    <workbookView xWindow="32760" yWindow="32760" windowWidth="24000" windowHeight="9555" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="造市折減(交易+結算)" sheetId="3" r:id="rId1"/>
     <sheet name="造市折減(交易經手費)" sheetId="1" r:id="rId2"/>
     <sheet name="造市折減(結算手續費)" sheetId="2" r:id="rId3"/>
+    <sheet name="保護基金提撥費用" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="30">
   <si>
     <t>SPF造市折減費用計算：</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -105,6 +105,50 @@
   </si>
   <si>
     <t>盤別</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPF保護基金費用計算：</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>UDF保護基金費用計算：</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>交易應收金額</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>結算應收金額</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>合計應收金額</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>提撥1%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>結算服務費累計(已扣除造市折減)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>其他折減費用(不含造市折減)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>結算應收金額</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>月份</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>月份</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -166,7 +210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -200,6 +244,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -209,23 +268,23 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1">
+    <xf numFmtId="176" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -246,7 +305,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1255,8 +1320,8 @@
   </sheetPr>
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:U65536"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1514,4 +1579,469 @@
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="47" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.875" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.5" style="11" customWidth="1"/>
+    <col min="10" max="10" width="9" style="3" customWidth="1"/>
+    <col min="11" max="11" width="11" style="3" customWidth="1"/>
+    <col min="12" max="12" width="9" style="3" customWidth="1"/>
+    <col min="13" max="13" width="15.875" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" style="3" customWidth="1"/>
+    <col min="15" max="15" width="35.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="31" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.875" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="1"/>
+      <c r="F1"/>
+      <c r="G1"/>
+      <c r="H1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="1"/>
+      <c r="O1"/>
+      <c r="P1"/>
+      <c r="Q1"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="4">
+        <f>SUM(D8:D9991)+SUM(H8:H65536)</f>
+        <v>0</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="1"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="1"/>
+      <c r="L2" s="4">
+        <f>SUM(M8:M9991)+SUM(Q8:Q65536)</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="1"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="4">
+        <f>ROUND(C2*1%,0)</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="1"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="4">
+        <f>ROUND(L2*1%,0)</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="2"/>
+      <c r="N3" s="1"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="1"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="1"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="1"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="1"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="1"/>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="8"/>
+      <c r="J7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q7" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H8" s="3">
+        <f>F8-G8</f>
+        <v>0</v>
+      </c>
+      <c r="Q8" s="3">
+        <f>O8-P8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H9" s="3">
+        <f t="shared" ref="H9:H31" si="0">F9-G9</f>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="3">
+        <f t="shared" ref="Q9:Q31" si="1">O9-P9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H10" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H11" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q11" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H12" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H13" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H14" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q14" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H15" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H16" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="H17" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q17" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="H18" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="H19" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="H20" s="3">
+        <f>F20-G20</f>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="3">
+        <f>O20-P20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="H21" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q21" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="H22" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q22" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="H23" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="H24" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="H25" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="H26" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q26" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="H27" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="H28" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q28" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="H29" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="H30" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q30" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="8:17" x14ac:dyDescent="0.25">
+      <c r="H31" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q31" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>